<commit_message>
📝 Update documentation document
</commit_message>
<xml_diff>
--- a/docs/GL/Product Backlog.xlsx
+++ b/docs/GL/Product Backlog.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26006"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26008"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_9248CACD84F5E813E97046798E3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3657126C-3B88-4444-A0BE-8C8E842D799D}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavasseur/Desktop/test/IUT/LP DAM/gp-dam-teamflexsante/docs/GL/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D984139C-BEAB-F142-86C8-8A3B51F14DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBD9E019-C25F-4A9C-83BE-08417F9D9ACE}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>Type of task</t>
   </si>
@@ -36,27 +41,60 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Use case</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UC 1</t>
+  </si>
+  <si>
+    <t>UC Register / Login / Logout</t>
+  </si>
+  <si>
     <t>CI / CD</t>
   </si>
   <si>
     <t>Task related to deployment...</t>
   </si>
   <si>
+    <t>UC 2</t>
+  </si>
+  <si>
+    <t>UC Health Data</t>
+  </si>
+  <si>
     <t>Task details</t>
   </si>
   <si>
+    <t>Use case related</t>
+  </si>
+  <si>
     <t>Backend</t>
   </si>
   <si>
     <t>Handle app logic + database</t>
   </si>
   <si>
+    <t>UC 3</t>
+  </si>
+  <si>
+    <t>UC Handle Personal Circle</t>
+  </si>
+  <si>
     <t>Init backend repository</t>
   </si>
   <si>
     <t>Frontend</t>
   </si>
   <si>
+    <t>UC 4</t>
+  </si>
+  <si>
+    <t>UC Handle Feeling Form</t>
+  </si>
+  <si>
     <t>Init frontend repository</t>
   </si>
   <si>
@@ -66,6 +104,12 @@
     <t>Create the user interface</t>
   </si>
   <si>
+    <t>UC 5</t>
+  </si>
+  <si>
+    <t>UC Insert Data</t>
+  </si>
+  <si>
     <t>UI for register page</t>
   </si>
   <si>
@@ -112,6 +156,24 @@
   </si>
   <si>
     <t>Create job to import health infos from sensor's API</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>UC 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> / UC 5</t>
+    </r>
   </si>
   <si>
     <t>UI for FeelingForm page</t>
@@ -148,18 +210,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -174,6 +231,64 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Corps)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -214,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -304,19 +419,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -339,6 +441,71 @@
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -346,28 +513,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,278 +864,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.75">
+    <row r="2" spans="2:11" ht="18.95">
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="F4" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="F4" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="H4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="18.75">
-      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="18.95">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="F6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="J6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="C29" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
✨ Update Diagrams & Specification document
- Update Authenticate Activity Diagram
- Update Specification document with updated activity diagram
</commit_message>
<xml_diff>
--- a/docs/GL/Product Backlog.xlsx
+++ b/docs/GL/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavasseur/Desktop/test/IUT/LP DAM/gp-dam-teamflexsante/docs/GL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D984139C-BEAB-F142-86C8-8A3B51F14DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBD9E019-C25F-4A9C-83BE-08417F9D9ACE}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D984139C-BEAB-F142-86C8-8A3B51F14DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA4A574-27A4-4101-8630-234C6D1A235A}"/>
   <bookViews>
     <workbookView xWindow="-3780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Type of task</t>
   </si>
@@ -129,6 +129,72 @@
   </si>
   <si>
     <t>User model</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">UC 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/ UC 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/ UC 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/ UC 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/ UC 5</t>
+    </r>
   </si>
   <si>
     <t>User authentication</t>
@@ -210,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +354,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -513,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -550,6 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +650,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -856,7 +938,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -867,7 +949,7 @@
   <dimension ref="B2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1040,8 +1122,8 @@
       <c r="C12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>4</v>
+      <c r="D12" s="36" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:11">
@@ -1049,7 +1131,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>4</v>
@@ -1060,7 +1142,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>4</v>
@@ -1071,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>4</v>
@@ -1082,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>4</v>
@@ -1093,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>4</v>
@@ -1104,7 +1186,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>4</v>
@@ -1115,7 +1197,7 @@
         <v>21</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>8</v>
@@ -1126,7 +1208,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>8</v>
@@ -1137,10 +1219,10 @@
         <v>12</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -1148,7 +1230,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>18</v>
@@ -1159,7 +1241,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>18</v>
@@ -1170,7 +1252,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D24" s="31" t="s">
         <v>18</v>
@@ -1181,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>14</v>
@@ -1192,7 +1274,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>14</v>
@@ -1203,7 +1285,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>14</v>
@@ -1214,7 +1296,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="34"/>
     </row>
@@ -1223,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" s="23"/>
     </row>
@@ -1232,7 +1314,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D30" s="23"/>
     </row>
@@ -1241,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D31" s="23"/>
     </row>

</xml_diff>

<commit_message>
📝 #105 Adding screenshots with progress into PO report and Product backlog
</commit_message>
<xml_diff>
--- a/docs/GL/Product Backlog.xlsx
+++ b/docs/GL/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavasseur/Desktop/test/IUT/LP DAM/gp-dam-teamflexsante/docs/GL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38453C07-E8ED-4CC5-B2EC-C3B010718F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{026B6CDB-ADB1-41F2-8A9E-6C2159705EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -912,6 +912,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF07DC79-1144-1F81-7FF5-09E89A31190F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9877425" y="3752850"/>
+          <a:ext cx="6124575" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1213,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:J7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1767,5 +1816,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📝 Update PO report
</commit_message>
<xml_diff>
--- a/docs/GL/Product Backlog.xlsx
+++ b/docs/GL/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavasseur/Desktop/test/IUT/LP DAM/gp-dam-teamflexsante/docs/GL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{026B6CDB-ADB1-41F2-8A9E-6C2159705EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03904B57-6E74-42D5-B848-5B3915C7E2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Type of task</t>
   </si>
@@ -263,6 +263,24 @@
     <t>HealthInfo page logic</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">UC 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/ UC 3</t>
+    </r>
+  </si>
+  <si>
     <t>#77</t>
   </si>
   <si>
@@ -339,7 +357,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +466,11 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF70AD47"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -829,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -896,6 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -920,21 +944,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2238375</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF07DC79-1144-1F81-7FF5-09E89A31190F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE9AE5E-749C-4915-93AA-47FA953ED02C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -950,8 +974,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9877425" y="3752850"/>
-          <a:ext cx="6124575" cy="2286000"/>
+          <a:off x="9877425" y="3952875"/>
+          <a:ext cx="5105400" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1262,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1614,11 +1638,11 @@
       <c r="C18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>40</v>
+      <c r="D18" s="66" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>12</v>
@@ -1629,13 +1653,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F19" s="46" t="s">
         <v>12</v>
@@ -1646,13 +1670,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20" s="46" t="s">
         <v>12</v>
@@ -1663,7 +1687,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" s="35" t="s">
         <v>48</v>
@@ -1676,7 +1700,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>48</v>
@@ -1689,7 +1713,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>48</v>
@@ -1702,7 +1726,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>44</v>
@@ -1715,7 +1739,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>44</v>
@@ -1728,7 +1752,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>44</v>
@@ -1741,7 +1765,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="9"/>
@@ -1752,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="9"/>
@@ -1763,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="9"/>
@@ -1774,7 +1798,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="26"/>
@@ -1782,14 +1806,14 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="40" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F31" s="46" t="s">
         <v>12</v>

</xml_diff>